<commit_message>
dataset reading bug detected
</commit_message>
<xml_diff>
--- a/Accuracy.xlsx
+++ b/Accuracy.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>Original</t>
   </si>
@@ -60,7 +60,7 @@
     <t>" له الفضل الاعظم في تطوير الموسيقى الكلاسيكية. بدا بيتهوفن يفقد سمعه في الثلاثينيات من عمره الا ان ذلك لم يؤثر على انتاجه الذي ازداد في تلك الفترة وتميز بالابداع.  اتسعت شهرته كعازف بيانو في سن مبكرة، ثم زاد انتاجه وذاع صيته كمؤلف موسيقى. في 1789 م تحقق حلمه اخيراً، فقد ارسله حاكم بون الى فيينا، وهناك تتلمذ على يد هايدن. فجاءت رسالته الى العالم كل البشر سيصبحون اخوة. "</t>
   </si>
   <si>
-    <t>"لودفيج فان بيتهوفن مؤلف موسيقي ألماني ولد عام 1770 م في مدينة بون.بدأ بيتهوفن يفقد سمعه في الثلاثينيات من عمره إلا أن ذلك لم يؤثر على إنتاجه الذي ازداد في تلك الفترة وتميز بالإبداع.شهدت مدينة بون الألمانية ميلاد الفنان العبقري لودفج فان بيتهوفن في 16 ديسمبر عام 1770، وتم تعميده في 17 ديسمبر 1770.ظهر تميزه الموسيقي منذ صغره، فنشرت أولى أعماله وهو في الثانية عشرمن عمره عام 1783 م. اتسعت شهرته كعازف بيانو في سن مبكرة، ثم زاد إنتاجه وذاع صيته كمؤلف موسيقى.في 1789 م تحقق حلمه أخيراً، فقد أرسله حاكم بون إلى فيينا، وهناك تتلمذ على يد هايدن.ولكن بيتهوفن، صاحب الألحان واجه بعض الخلافات مع معلمه، وعندما سافر هايدن إلى لندن، تحول بيتهوفن إلى معلمين آخرين مثل ساليري وشينك وألبريشتبيرجر.وحاول أن يشق لنفسه طريق كعازف في عاصمة الموسيقى، وسرعان ما لاقى مكانة كبرى خاصة في الأوساط الأرستقراطية.بدأت إصابة بيتهوفن بصمم بسيط عام 1802، فبدأ في الانسحاب من الأوساط الفنية تدريجياً، وأمضى حياته بلا زواج يرتبط بعلاقات عدة مع سيدات صغيرات.ومع ازدياد حالة الصمم التي أصابته، امتنع عن العزف في الحفلات العامة، وابتعد عن الحياة الاجتماعية واتجه للوحدة، وقلت مؤلفاته، وأصبحت أكثر تعقيداً.وبالفعل مازالت أعماله حتى اليوم من أهم ما أنتجته الموسيقى الكلاسيكية العالمية.</t>
+    <t>بيتهوفن يفقد سمعه في الثلاثينيات من عمره إلا أن ذلك لم يؤثر على إنتاجه الذي ازداد في تلك الفترة وتميز بالإبداع.مدينة بون الألمانية ميلاد الفنان العبقري لودفج فان بيتهوفن في 16 ديسمبر عام 1770، وتم تعميده في 17 ديسمبر 1770.ظهر تميزه الموسيقي منذ صغره، فنشرت أولى أعماله وهو في الثانية عشرمن عمره عام 1783 م. اتسعت شهرته كعازف بيانو في سن مبكرة، ثم زاد إنتاجه وذاع صيته كمؤلف موسيقى.1789 م تحقق حلمه أخيراً، فقد أرسله حاكم بون إلى فيينا، وهناك تتلمذ على يد هايدن.ولكن بيتهوفن، صاحب الألحان واجه بعض الخلافات مع معلمه، وعندما سافر هايدن إلى لندن، تحول بيتهوفن إلى معلمين آخرين مثل ساليري وشينك وألبريشتبيرجر.وحاول أن يشق لنفسه طريق كعازف في عاصمة الموسيقى، وسرعان ما لاقى مكانة كبرى خاصة في الأوساط الأرستقراطية.إصابة بيتهوفن بصمم بسيط عام 1802، فبدأ في الانسحاب من الأوساط الفنية تدريجياً، وأمضى حياته بلا زواج يرتبط بعلاقات عدة مع سيدات صغيرات.ومع ازدياد حالة الصمم التي أصابته، امتنع عن العزف في الحفلات العامة، وابتعد عن الحياة الاجتماعية واتجه للوحدة، وقلت مؤلفاته، وأصبحت أكثر تعقيداً.وبالفعل مازالت أعماله حتى اليوم من أهم ما أنتجته الموسيقى الكلاسيكية العالمية.</t>
   </si>
   <si>
     <t>الناي آلة نفخية تعد بحق أقدم آلة موسيقية في التاريخ ( إذا استثنينا الآلات الإيقاعية ( وللناي عدة أسماء تعرف بها منها الناي القصبة الشبابة المنجيرة . والناي كلمة فارسية تعني المزمار . هي قصبة مفتوحة الطرفين يعزف عليها بواسطة وضع الفم على أحد طرفيها مع إمالته قليلا بزاوية مما يجعل الهواء يصطدم بجدارها الداخلي مصدرا بالنتيجة صوتا شجيا هو أقرب الأصوات وأجملها بالنسبة للإنسان .وللناي ستة ثقوب ( وأحيانا سبعه ) وثقب في منتصف القصبة من الأسفل. وتسد هذه الثقوب وتفتح حسب درجة الصوت ولإخراج العلامات بتسلسل يستطيع معه العازف إخراج العلامات الموسيقية لإخراج اللحن المطلوب . والثقب الخلفي يسد بالإبهام ويستخدم لإظهار جواب العلامة الدنيا التي تظهر في البداية . وتحتاج هذه الآلة إلى براعة شديدة حيث لها 3 تقنيات.التقنية الأولى : هي طريقة النفخ حيث أن إخراج الصوت الطبيعي منها هي أول صعوبة يجب التغلب عليها لمن أراد التعلم عليها . لذلك ينصح عادة بأن يتمرن من يريد التعلم بالتدريب على إخراج الصوت أولا ومن ثم عندما يستطيع ذلك يبدأ بالتعلم على إخراج الدرجات الصوتية ( تمرين الأصابع ) . والعازف الخبير يستطيع بتغيير طريقة النفخ التلاعب بهذه الآلة الخطيرة حيث يستطيع العازف المتمكن أن يخرج أكثر من سبع علامات صحيحة أو حتى أكتر من أوكتاف ( ديوان ) فالآلة تنتج 7 أصوات صحيحة تماما وبالتالي يستطيع العازف الخبير أن ينتج 7 أصوات أخفض و 7 أصوات أعلى . التقنية الثانية : هي إمالة الشبابة بأكثر من زاوية لإخراج أصوات معينة أو ربع التون . التقنية الثالثة : وهي طريقة سد الثقوب بحيث ينتج الأصوات المطلوبة أو سد الثقوب بطريقة معينة لإنتاج ربع التون ( العلامات الشرقية ) . وآلة الناي آلة أساسية في التخت الشرقي التقليدي حيث أن صوتها قريب جدا إلى الأذن البشرية .وقد اعتاد إخواننا المصريين إضافة عدة آلات تشبهها بالطريقة ( مع الاختلاف بطبيعة الصوت ) ومنها آلة الكولة ولكنهم لم يلغوا هذه الآلة العظيمة . عيوب هذه الآلة كثيرة أبرزها أن صوتها ليس ثابتا لذلك تعتمد كثيرا على أذن العازف الذي يجب ان يكون بارعا وذو أذن صافية ممتازة حتى تؤدي دورها الصحيح . والعيب الثاني أن لكل ناي درجة صوتية يبدأ منها ولذلك تجد أن العازف عادة ما يملك أكثر من ناي وعادة ما يكون عددها سبع وإن كان بعض العازفين المهرة جدا يكتفون بأربع أو ثلاث قصبات ويتحايلون على بقية المقامات.</t>
@@ -69,7 +69,7 @@
     <t xml:space="preserve">الناي آلة نفخية تعد بحق اقدم آلة موسيقية في التاريخ ( اذا استثنينا الآلات الايقاعية ( وللناي عدة اسماء تعرف بها منها الناي القصبة الشبابة المنجيرة . التقنية الاولى : هي طريقة النفخ حيث ان اخراج الصوت الطبيعي منها هي اول صعوبة يجب التغلب عليها لمن اراد التعلم عليها .  والعازف الخبير يستطيع بتغيير طريقة النفخ التلاعب بهذه الآلة الخطيرة حيث يستطيع العازف المتمكن ان يخرج اكثر من سبع علامات صحيحة او حتى اكتر من اوكتاف ( ديوان ) فالآلة تنتج 7 اصوات صحيحة تماما وبالتالي يستطيع العازف الخبير ان ينتج 7 اصوات اخفض و 7 اصوات اع.  التقنية الثانية : هي امالة الشبابة باكثر من زاوية لاخراج اصوات معينة او ربع التون .  التقنية الثالثة : وهي طريقة سد الثقوب بحيث ينتج الاصوات المطلوبة او سد الثقوب بطريقة معينة لانتاج ربع التون ( العلامات الشرقية ) . وقد اعتاد اخواننا المصريين اضافة عدة آلات تشبهها بالطريقة ( مع الاختلاف بطبيعة الصوت ) ومنها آلة الكولة ولكنهم لم يلغوا هذه الآلة العظيمة .  عيوب هذه الآلة كثيرة ابرزها ان صوتها ليس ثابتا لذلك تعتمد كثيرا على اذن العازف الذي يجب ان يكون بارعا وذو اذن صافية ممتازة حتى تؤدي دورها الصحيح .  والعيب الثاني ان لكل ناي درجة صوتية يبدا منها ولذلك تجد ان العازف عادة ما يملك اكثر من ناي وعادة ما يكون عددها سبع وان كان بعض العازفين المهرة جدا يكتفون باربع او ثلاث قصبات ويتحايلون على بقية المقامات. </t>
   </si>
   <si>
-    <t>الناي آلة نفخية تعد بحق أقدم آلة موسيقية في التاريخ ( إذا استثنينا الآلات الإيقاعية ( وللناي عدة أسماء تعرف بها منها الناي القصبة الشبابة المنجيرة .هي قصبة مفتوحة الطرفين يعزف عليها بواسطة وضع الفم على أحد طرفيها مع إمالته قليلا بزاوية مما يجعل الهواء يصطدم بجدارها الداخلي مصدرا بالنتيجة صوتا شجيا هو أقرب الأصوات وأجملها بالنسبة للإنسان .والعازف الخبير يستطيع بتغيير طريقة النفخ التلاعب بهذه الآلة الخطيرة حيث يستطيع العازف المتمكن أن يخرج أكثر من سبع علامات صحيحة أو حتى أكتر من أوكتاف ( ديوان ) فالآلة تنتج 7 أصوات صحيحة تماما وبالتالي يستطيع العازف الخبير أن ينتج 7 أصوات أخفض و 7 أصوات أعلى .عيوب هذه الآلة كثيرة أبرزها أن صوتها ليس ثابتا لذلك تعتمد كثيرا على أذن العازف الذي يجب ان يكون بارعا وذو أذن صافية ممتازة حتى تؤدي دورها الصحيح .والعيب الثاني أن لكل ناي درجة صوتية يبدأ منها ولذلك تجد أن العازف عادة ما يملك أكثر من ناي وعادة ما يكون عددها سبع وإن كان بعض العازفين المهرة جدا يكتفون بأربع أو ثلاث قصبات ويتحايلون على بقية المقامات.</t>
+    <t>الناي آلة نفخية تعد بحق أقدم آلة موسيقية في التاريخ ( إذا استثنينا الآلات الإيقاعية ( وللناي عدة أسماء تعرف بها منها الناي القصبة الشبابة المنجيرة .هي قصبة مفتوحة الطرفين يعزف عليها بواسطة وضع الفم على أحد طرفيها مع إمالته قليلا بزاوية مما يجعل الهواء يصطدم بجدارها الداخلي مصدرا بالنتيجة صوتا شجيا هو أقرب الأصوات وأجملها بالنسبة للإنسان .وللنايوالعازف الخبير يستطيع بتغيير طريقة النفخ التلاعب بهذه الآلة الخطيرة حيث يستطيع العازف المتمكن أن يخرج أكثر من سبع علامات صحيحة أو حتى أكتر من أوكتاف ( ديوان ) فالآلة تنتج 7 أصوات صحيحة تماما وبالتالي يستطيع العازف الخبير أن ينتج 7 أصوات أخفض و 7 أصوات أعلى .عيوب هذه الآلة كثيرة أبرزها أن صوتها ليس ثابتا لذلك تعتمد كثيرا على أذن العازف الذي يجب ان يكون بارعا وذو أذن صافية ممتازة حتى تؤدي دورها الصحيح .والعيب الثاني أن لكل ناي درجة صوتية يبدأ منها ولذلك تجد أن العازف عادة ما يملك أكثر من ناي وعادة ما يكون عددها سبع وإن كان بعض العازفين المهرة جدا يكتفون بأربع أو ثلاث قصبات ويتحايلون على بقية المقامات.</t>
   </si>
   <si>
     <t>"العود هي آلة موسيقية شرقية وترية تاريخها موغل بالقدم يرجعه البعض إلى نوح.و تعني كلمة العود في اللغة العربية الخشب .فالعود من الآلات الوترية العربية له خمسة أوتار ثنائية أو و يمكن ربط وتر سادس إلى العود و يغطي مجاله الصوتي حوالي الأوكتافين و نصف الأوكتاف.الأدبيات الشرقيةالموسيقية كلها تظهر وتؤكد على استخدام نوع أو أكثر من الأعواد.يعتبر العود آلة رئيسية في التخت الموسيقي الشرقي</t>
@@ -78,7 +78,7 @@
     <t xml:space="preserve"> في التاريخ الحديث هناك أكثر من دولة عربية تدعي تفوقها في صناعة الأعواد ولكن بغداد لها السبق في ذلك ففي بغداد هناك أكثر من حرفي يفوم بصنعها</t>
   </si>
   <si>
-    <t>"العود هي آلة موسيقية شرقية وترية تاريخها موغل بالقدم يرجعه البعض إلى نوح.</t>
+    <t>"العود هي آلة موسيقية شرقية وترية تاريخها موغل بالقدم يرجعه البعض إلى نوح.و تعني كلمة العود في اللغة العربية الخشب .فالعود</t>
   </si>
   <si>
     <t>" الخطاط الكويتي فريد العلي يعرض مجموعة محمديات بدعوة من جمعية العلوم الاجتماعية وتحت رعاية عميد كلية العلوم الاجتماعيةالدكتور علي الطراح افتتحت الدكتورة نادية الحمدان رئيس مكتب التوجيه والإرشادمعرض (خير الأنام)</t>
@@ -111,7 +111,7 @@
     <t>"وتضمنت شروط المسابقة، تنظيم مسابقة رسم للاطفال حول موضوع «عام الكيخوتي» حيثبامكان جميع الاطفال الذين تتراوح اعمارهم ما بين 4 و12 سنة من المقيمين في عماناو في مدن المملكة الاخرى المشاركة فيها. cervantes. es] طيلة فترة العام الدراسي الحالي. - كل مشارك سيُمنح مشاركة وتذكارا تعبيرا عن امتناننا لمشاركته. "</t>
   </si>
   <si>
-    <t>" عمان- الرأي- دعا معهد ثربانتس بعمان للمشاركة بمسابقة الرسم الاولى للاطفالالمقيمين في الاردن والذين تتراوح اعمارهم ما بين 4 و12 سنة، وعنوان مسابقة الرسمهو «عام الكيخوتي».وتضمنت شروط المسابقة، تنظيم مسابقة رسم للاطفال حول موضوع «عام الكيخوتي» حيثبامكان جميع الاطفال الذين تتراوح اعمارهم ما بين 4 و12 سنة من المقيمين في عماناو في مدن المملكة الاخرى المشاركة فيها.كل طفل مشارك في المسابقة يستطيع تقديمرسمة او رسمتين كحد اقصى، وله مطلق الحرية في اختيار اداة الرسم سواء كانت اقلاماخشبية او الوانا شمعية او الوان مائية او كولاجا او معاجين لطيفة، الخ.. ، على انتكون بحجم الورقة الطبيعية A4 واقصاه ضعف الحجم الطبيعي للورقة العادية اي A3. وجاءت قواعد المشاركة وموعد تسليم الرسومات كالآتي:- تُرسل الرسومات او تُسلم بصفة شخصية الى سكرتارية معهد ثربانتس في عمان قبل يوم23 ايار 2005.- ستُعرض الرسومات في صالة معارض معهد ثربانتس، والرسومات الفائزة ستُنشر علىصفحة الويب الخاصة بمعهد ثربانتس في عمان http://amman.cervantes.</t>
+    <t>" عمان- الرأي- دعا معهد ثربانتس بعمان للمشاركة بمسابقة الرسم الاولى للاطفالالمقيمين في الاردن والذين تتراوح اعمارهم ما بين 4 و12 سنة، وعنوان مسابقة الرسمهو «عام الكيخوتي».وتضمنتشروط المسابقة، تنظيم مسابقة رسم للاطفال حول موضوع «عام الكيخوتي» حيثبامكان جميع الاطفال الذين تتراوح اعمارهم ما بين 4 و12 سنة من المقيمين في عماناو في مدن المملكة الاخرى المشاركة فيها.كل طفل مشارك في المسابقة يستطيع تقديمرسمة او رسمتين كحد اقصى، وله مطلق الحرية في اختيار اداة الرسم سواء كانت اقلاماخشبية او الوانا شمعية او الوان مائية او كولاجا او معاجين لطيفة، الخ..، على انتكون بحجم الورقة الطبيعية A4 واقصاه ضعف الحجم الطبيعي للورقة العادية اي A3.وجاءت قواعد المشاركة وموعد تسليم الرسومات كالآتي:- تُرسل الرسومات او تُسلم بصفة شخصية الى سكرتارية معهد ثربانتس في عمان قبل يوم23 ايار 2005.- ستُعرض الرسومات في صالة معارض معهد ثربانتس، والرسومات الفائزة ستُنشر علىصفحة الويب الخاصة بمعهد ثربانتس في عمان http://amman.cervantes.es[http://amman.cervantes.es]</t>
   </si>
   <si>
     <t xml:space="preserve">"نجيب محفوظ هو نجيب محفوظ بن عبد العزيز بن إبراهيم بن أحمد باشا. اسمه المفرد مركب من اسمين تقديراً من والده للطبيب الراحل نجيب محفوظ الذى أشرف على ولادته. روائي مصري حائز على جائزة نوبل في الآداب عام 1988م. ولد في القاهرة، وحصل على ليسانس الآداب قسم الفلسفة من جامعة القاهرة وتدرج بالوظائف الحكومية حتى عمل مديرا عاما للرقابة على المصنفات الفنية عام 1959م. تعرض محفوظ للهجوم و المنع من قبل بعض الإسلاميين المتطرفين الذين رأوا في كتاباته مساسا بالشخصيات الدينية، خصوصا بسبب روايته أولاد حارتنا التي منعت من الطبع في مصر حتى نهاية عام 2006، حيث يستخدم محفوظ الرموز الشعبية ليقدم شخصيات الانبياء. وتعرض إلى محاولة اغتيال فاشلة عام 1994. بدأ نجيب محفوظ بكتابة الرواية التاريخية ثم الرواية الأجتماعية. وتزيد مؤلفاته على 50 مؤلفاً. ترجمت معظم أعماله إلى العديد من اللغات العالمية وحصل على جائزة الدولة التشجيعية في الروايةعام 1959.أتم دراسته الإبتدائية والثانوية و عمره 18 سنة. وقد التحق بالجامعة سنة 1930م ثم حصل على الليسانس في الفلسفة. يعد نجيب محفوظ من الادباء العباقرة في مجال الرواية وقد وهب حياته كلها لهذا العمل، كما انه يتميز بالقدرة الكبيرة على التفاعل مع القضايا المحيطة به، واعادة انتاجها على شكل ادب يربط الناس بما يحصل في المراحل العامة التي عاشتها مصر. يتميز اسلوب محفوظ بالبساطة، والقرب من الناس كلهم، لذلك اصبح بحق الروائي العربي الاكثر شعبية . رغم إن نجيب قد انخرط في عدة أعمال إلا أن العمل الذي التهم حياته هو الكتابة. فقد كتب في مجلة الرسالة قصصا صغيرة و من أشهر أساتذتة سلامة موسى بالاضافة إلى ذلك فقد شرع نجيب محفوظ في اعداد رسالة المجاستير تحت اشراف استاذه الشيخ مصطفى عبد الرازق وكانت في الفلسفة وموضوعها هو  الجمال في الفلسفة الإسلامية  بيد أن الأدب كان قد جرفه في طريقه .. وشعر محفوظ بالتمزق والتشتت بين الفلسفة التي يدرسها والأدب الذي يهواه وملك عليه لبه ؛ ثم انقذه من هذه الحيرة اتخاذه قرارا نهائيا بالاعتذار عن اكمال الرسالة ليتفرغ للأدب . وهذا ما حدث بالفعل.وقد ساعده استاذه سلامة موسى على نشر أولى رواياته وهي  عبث الأقدار .أما أول مجموعة قصصية نشرت له فكانت  همس الجنون  حيث انتقى بعضا من قصصه القصيرة </t>
@@ -120,7 +120,7 @@
     <t xml:space="preserve"> ونشرت في هذه المجموعة . وبعض هذه القصص التي كتبها في تلك الفترة  فترة الثلاثينيات والأربعينيات  اعدها للنشر في عام 2005 الأديب محمد جبريل في مجموعة تحت عنوان  فتوة العطوف .توفي في الثامنة وخمس دقائق من صباح الأربعاء 30 أغسطس 2006 م في مستشفى الشرطة بحي العجوزة وسط القاهرة وذكر مصدر طبي أن محفوظ توفي في وحدة العناية المركزة جراء قرحة نازفة بعدما أصيب بهبوط مفاجئ في ضغط الدم وفشل كلوي. وكان الروائي الشهير قد أدخل في يوليو 2005 المستشفى ذاته إثر سقوطه في الشارع وإصابته بجرح غائر في الرأس تطلب جراحة فورية. وظل نجيب محفوظ حتى أيامه الأخيرة حريصا على برنامجه اليومي في الالتقاء بأصدقائه في بعض فنادق القاهرة، حيث كانوا يقرؤون له عناوين الأخبار ويستمعون إلى تعليقاته على الأحداث."</t>
   </si>
   <si>
-    <t>اسمه المفرد مركب من اسمين تقديراً من والده للطبيب الراحل نجيب محفوظ الذى أشرف على ولادته.ولد في القاهرة، وحصل على ليسانس الآداب قسم الفلسفة من جامعة القاهرة وتدرج بالوظائف الحكومية حتى عمل مديرا عاما للرقابة على المصنفات الفنية عام 1959م.تعرض محفوظ للهجوم و المنع من قبل بعض الإسلاميين المتطرفين الذين رأوا في كتاباته مساسا بالشخصيات الدينية، خصوصا بسبب روايته أولاد حارتنا التي منعت من الطبع في مصر حتى نهاية عام 2006، حيث يستخدم محفوظ الرموز الشعبية ليقدم شخصيات الانبياء.ترجمت معظم أعماله إلى العديد من اللغات العالمية وحصل على جائزة الدولة التشجيعية في الروايةعام 1959.يعد نجيب محفوظ من الادباء العباقرة في مجال الرواية وقد وهب حياته كلها لهذا العمل، كما انه يتميز بالقدرة الكبيرة على التفاعل مع القضايا المحيطة به، واعادة انتاجها على شكل ادب يربط الناس بما يحصل في المراحل العامة التي عاشتها مصر.يتميز اسلوب محفوظ بالبساطة، والقرب من الناس كلهم، لذلك اصبح بحق الروائي العربي الاكثر شعبية .</t>
+    <t>ولد في القاهرة، وحصل على ليسانس الآداب قسم الفلسفة من جامعة القاهرة وتدرج بالوظائف الحكومية حتى عمل مديرا عاما للرقابة على المصنفات الفنية عام 1959م.تعرض محفوظ للهجوم و المنع من قبل بعض الإسلاميين المتطرفين الذين رأوا في كتاباته مساسا بالشخصيات الدينية، خصوصا بسبب روايته أولاد حارتنا التي منعت من الطبع في مصر حتى نهاية عام 2006، حيث يستخدم محفوظ الرموز الشعبية ليقدم شخصيات الانبياء.ترجمت معظم أعماله إلى العديد من اللغات العالمية وحصل على جائزة الدولة التشجيعية في الروايةعام 1959.أتم دراسته الإبتدائية والثانوية و عمره 18 سنة.يعد نجيب محفوظ من الادباء العباقرة في مجال الرواية وقد وهب حياته كلها لهذا العمل، كما انه يتميز بالقدرة الكبيرة على التفاعل مع القضايا المحيطة به، واعادة انتاجها على شكل ادب يربط الناس بما يحصل في المراحل العامة التي عاشتها مصر.يتميز اسلوب محفوظ بالبساطة، والقرب من الناس كلهم، لذلك اصبح بحق الروائي العربي الاكثر شعبية .</t>
   </si>
   <si>
     <t>"فيروز اسمها الأصلي نهاد وديع حداد، مطربة لبنانية تعد من أشهر الفنانين العرب على قيد الحياة. شكلت مع زوجها الراحل عاصي الرحباني وأخوه منصور الرحبانيالمعروفين بالأخوين رحباني ثورة في عالم الموسيقى والغناء العربي.كانت انطلاقتها عام 1952 م عندما بدأت الغناء لعاصي الرحباني، وكانت الأغاني التي غنّتها لعاصي في ذلك الوقت تملأ كافة القنوات الإذاعية، وأصبحت مطربة كبيرة في العالم العربي منذ ذلك الوقت. كانت أغلب أغانيها آنذك للأخوين عاصي ومنصور الرحباني الذين يشار لهما دائما بالأخوين رحباني. وفي 1955م تزوجت فيروز من عاصي الرحباني، وأنجبت منه زياد عام 1956 ثم هالي وهو مقعد وانجبته عام 1958 ثم ليال عام 1960 واخيرا ريما عام 1965.قدم الأخوين رحباني مع فيروز المئات من الأغاني التي أحدثت ثورة في الموسيقى العربية، لتميزها بقصر المدة وقوة المعنى على عكس الأغاني العربية السائدة في ذلك الحين والتي كانت تمتاز بالطول وبساطة التعبير وعمق الفكرة الموسيقية وتنوع المواضيع، حيث غنت فيروز الحب والأطفال، الحزن والفرح، الوطن، الأم. وقدّم عدد كبير من هذه الأغاني ضمن مجموعة مسرحيات من تأليف وتلحين الأخوين رحباني وصل عددها إلى اثنتي عشر مسرحية. تنوعت مواضيعها بين نقد الحاكم والشعب وتمجيد البطولة والحب بشتى أنواعه.غنت فيروز لعديد من الشعراء والملحنين، وأمام العديد من الملوك والرؤساء، وفي أغلب المهرجانات الكبرى في العالم العربي. وأطلق عليها عدة ألقاب منها سفيرتنا إلى النجوم للدلالة على رقي صوتها وتميزه.بعد وفاة زوجها عاصي عام 1986، خاضت تجارب عديدة مع مجموعة ملحنين ومؤلفين من أبرزهم فلمون وهبة و زكي ناصيف، لكنها عملت بشكل رئيسي مع ابنها زياد الرحباني الذي قدم لها مجموعة كبيرة من الأغاني أبرزت موهبته وقدرته على خلق نمط موسيقي خاص به يستقي من الموسيقا العربية والموسيقا العالمية، وما زالت مسيرة الفنانين مستمرة بنجاح حتى يومنا هذا. تجلت هذه المرحلة بالعديد من الألبومات من أبرزها كيفك انت، فيروز في بيت الدين 2000 والذي كان تسجيلاً حياً من مجموعة حفلات أقامتها فيروز بمصاحبة ابنها زياد وأوركسترا تضم عازفين أرمن وسوريين ولبنانيين، وكانت البداية لسلسلة حفلات حظيت بنجاح منقطع النظير لما قدمته من جديد على صعيد التوزيع الموسيقي والتنوع في الأغاني بين القديمة والحديثة ، ألبوم ولا كيف عام 2001 كان آخر ما قدمته فيروز من تسجيل، وجميع عشاقها في انتظار ألبوم جديد طال الحديث عنه، ومن المرجح أن تأخره عائد إلى الأوضاع الحرجه في لبنان في الآونة الأخيرة."</t>
@@ -129,7 +129,7 @@
     <t>"فيروز اسمها الاصلي نهاد وديع حداد، مطربة لبنانية تعد من اشهر الفنانين العرب على قيد الحياة.  شكلت مع زوجها الراحل عاصي الرحباني واخوه منصور الرحبانيالمعروفين بالاخوين رحباني ثورة في عالم الموسيقى والغناء العربي. كانت انطلاقتها عام 1952 م عندما بدات الغناء لعاصي الرحباني، وكانت الاغاني التي غنّتها لعاصي في ذلك الوقت تملا كافة القنوات الاذاعية، واصبحت مطربة كبيرة في العالم العربي منذ ذلك الوقت.  كانت اغلب اغانيها آنذك للاخوين عاصي ومنصور الرحباني الذين يشار لهما دائما بالاخوين رحباني. غنت فيروز لعديد من الشعراء والملحنين، وامام العديد من الملوك والرؤساء، وفي اغلب المهرجانات الكبرى في العالم العربي. قدم الاخوين رحباني مع فيروز المئات من الاغاني التي احدثت ثورة في الموسيقى العربية، لتميزها بقصر المدة وقوة المعنى على عكس الاغاني العربية السائدة في ذلك الحين والتي كانت تمتاز بالطول وبساطة التعبير وعمق الفكرة الموسيقية وتنوع المواضيع، حيث غنت فيروز الحب . "</t>
   </si>
   <si>
-    <t>وفي 1955م تزوجت فيروز من عاصي الرحباني، وأنجبت منه زياد عام 1956 ثم هالي وهو مقعد وانجبته عام 1958 ثم ليال عام 1960 واخيرا ريما عام 1965.قدم الأخوين رحباني مع فيروز المئات من الأغاني التي أحدثت ثورة في الموسيقى العربية، لتميزها بقصر المدة وقوة المعنى على عكس الأغاني العربية السائدة في ذلك الحين والتي كانت تمتاز بالطول وبساطة التعبير وعمق الفكرة الموسيقية وتنوع المواضيع، حيث غنت فيروز الحب والأطفال، الحزن والفرح، الوطن، الأم.بعد وفاة زوجها عاصي عام 1986، خاضت تجارب عديدة مع مجموعة ملحنين ومؤلفين من أبرزهم فلمون وهبة و زكي ناصيف، لكنها عملت بشكل رئيسي مع ابنها زياد الرحباني الذي قدم لها مجموعة كبيرة من الأغاني أبرزت موهبته وقدرته على خلق نمط موسيقي خاص به يستقي من الموسيقا العربية والموسيقا العالمية، وما زالت مسيرة الفنانين مستمرة بنجاح حتى يومنا هذا.تجلت هذه المرحلة بالعديد من الألبومات من أبرزها كيفك انت، فيروز في بيت الدين 2000 والذي كان تسجيلاً حياً من مجموعة حفلات أقامتها فيروز بمصاحبة ابنها زياد وأوركسترا تضم عازفين أرمن وسوريين ولبنانيين، وكانت البداية لسلسلة حفلات حظيت بنجاح منقطع النظير لما قدمته من جديد على صعيد التوزيع الموسيقي والتنوع في الأغاني بين القديمة والحديثة ، ألبوم ولا كيف عام 2001 كان آخر ما قدمته فيروز من تسجيل، وجميع عشاقها في انتظار ألبوم جديد طال الحديث عنه، ومن المرجح أن تأخره عائد إلى الأوضاع الحرجه في لبنان في الآونة الأخيرة.</t>
+    <t>وفي 1955م تزوجت فيروز من عاصي الرحباني، وأنجبت منه زياد عام 1956 ثم هالي وهو مقعد وانجبته عام 1958 ثم ليال عام 1960 واخيرا ريما عام 1965.قدم الأخوين رحباني مع فيروز المئات من الأغاني التي أحدثت ثورة في الموسيقى العربية، لتميزها بقصر المدة وقوة المعنى على عكس الأغاني العربية السائدة في ذلك الحين والتي كانت تمتاز بالطول وبساطة التعبير وعمق الفكرة الموسيقية وتنوع المواضيع، حيث غنت فيروز الحب والأطفال، الحزن والفرح، الوطن، الأم.وفاة زوجها عاصي عام 1986، خاضت تجارب عديدة مع مجموعة ملحنين ومؤلفين من أبرزهم فلمون وهبة و زكي ناصيف، لكنها عملت بشكل رئيسي مع ابنها زياد الرحباني الذي قدم لها مجموعة كبيرة من الأغاني أبرزت موهبته وقدرته على خلق نمط موسيقي خاص به يستقي من الموسيقا العربية والموسيقا العالمية، وما زالت مسيرة الفنانين مستمرة بنجاح حتى يومنا هذا.تجلت هذه المرحلة بالعديد من الألبومات من أبرزها كيفك انت، فيروز في بيت الدين 2000 والذي كان تسجيلاً حياً من مجموعة حفلات أقامتها فيروز بمصاحبة ابنها زياد وأوركسترا تضم عازفين أرمن وسوريين ولبنانيين، وكانت البداية لسلسلة حفلات حظيت بنجاح منقطع النظير لما قدمته من جديد على صعيد التوزيع الموسيقي والتنوع في الأغاني بين القديمة والحديثة ، ألبوم ولا كيف عام 2001 كان آخر ما قدمته فيروز من تسجيل، وجميع عشاقها في انتظار ألبوم جديد طال الحديث عنه، ومن المرجح أن تأخره عائد إلى الأوضاع الحرجه في لبنان في الآونة الأخيرة."</t>
   </si>
   <si>
     <t>"لوتشانو بافاروتي مواليد مودينا في 12 أكتوبر 1935 -توفي بمودينا في 6 سبتمبر 2007، مغني تينور إيطالي، يعد من أشهر فنانين الأوبرا في الطبقة العالية من الرجال في عصرنا الحاضر، وأحد التينور الثلاثة وقد ولد في مدينة مودينا . ولد في بمدينة مودينا شمال إيطاليا لعائلة خباز، بعد أن تخلى عن حلمه بأن يصبح حارس مرمى كرة قدم محترف،ثم قضاء سبعة سنوات في التدريب الصوتى، بدأ بافاروتي حياته كتينور في إيطاليا عام 1961، ثم بدأ الغناء في دور الأوبرا فيهولندا و فيينا ولندنوأنقرةوبودابستوبرشلونة. وقد اكتسب التينور الشاب حينها الخبرة القيمة بالإضافة إلى التقدير الواضح.وفى أثناء عروضه للولايات المتحدة على دعوة من السوبرانوساثرلاندعام 1965 زاع صيته وثبت أقدامه على الساحة العالمية بين عامى 1966 و1972 حيث أدى في أكبر دور الأوبرا في العالم مثل La Scalaفى ميلان. بحلول منتصف السبعينيات، صار بافاروتي مشهورا في جميع أنحاء العالم بتميز وروعة صوته خاصة الطبقات العليا. وبين عامى 1970 و1980 كان بافاروتي قد اثبت نفسه كأحد أعظم مطربي التينور بعروضه المتعددة في أكبر دور الأوبرا في العالم. كما زاع صيته خارج نطاق جمهور الأوبرا كنجم غنائي في عام كأس العالم بإيطاليا خاصة بعد أدائه الرائعة لأريا Nessun Dormaمن أوبراTurandot كأحد التينور الثلاثة في حفلهم الأول عشية نهائي كأس العالم، غنى فيها بافاروتي مع نجمي التينور بلاسيدو دومينجو وخوسيه كاريراس ومعا حققوا شهرة طاغية ونجاحا عظيما في جميع أنحاء العالم. السنوات التالية لاقت تقلصا في عدد أدائه للأوبرات على المسرح بسبب الزيادة المفرطة في وزنه وكان أخر أداء في أوبرا له في مارس عام 2004 في Mets. وفى الأوليمبيات الشتوية في تورينو Turinعام 2006 شاهدته إيطاليا والعالم يغنى للمرة الأخيرة حيث غنى بافاروتي Nessun Dorma وأدت الجموع الكبيرة دور الكورال المصاحب، في أداء مهيب مؤثر."</t>
@@ -138,7 +138,7 @@
     <t>"لوتشانو بافاروتي مواليد مودينا في 12 اكتوبر 1935 -توفي بمودينا في 6 سبتمبر 2007، مغني تينور ايطالي، يعد من اشهر فنانين الاوبرا في الطبقة العالية من الرجال في عصرنا الحاضر، واحد التينور الثلاثة وقد ولد في مدينة مودينا . "</t>
   </si>
   <si>
-    <t>"لوتشانو بافاروتي مواليد مودينا في 12 أكتوبر 1935 -توفي بمودينا في 6 سبتمبر 2007، مغني تينور إيطالي، يعد من أشهر فنانين الأوبرا في الطبقة العالية من الرجال في عصرنا الحاضر، وأحد التينور الثلاثة وقد ولد في مدينة مودينا .ولد في بمدينة مودينا شمال إيطاليا لعائلة خباز، بعد أن تخلى عن حلمه بأن يصبح حارس مرمى كرة قدم محترف،ثم قضاء سبعة سنوات في التدريب الصوتى، بدأ بافاروتي حياته كتينور في إيطاليا عام 1961، ثم بدأ الغناء في دور الأوبرا فيهولندا و فيينا ولندنوأنقرةوبودابستوبرشلونة.وقد اكتسب التينور الشاب حينها الخبرة القيمة بالإضافة إلى التقدير الواضح.</t>
+    <t>"لوتشانو بافاروتي مواليد مودينا في 12 أكتوبر 1935 -توفي بمودينا في 6 سبتمبر 2007، مغني تينور إيطالي، يعد من أشهر فنانين الأوبرا في الطبقة العالية من الرجال في عصرنا الحاضر، وأحد التينور الثلاثة وقد ولد في مدينة مودينا .ولد في بمدينة مودينا شمال إيطاليا لعائلة خباز، بعد أن تخلى عن حلمه بأن يصبح حارس مرمى كرة قدم محترف،ثم قضاء سبعة سنوات في التدريب الصوتى، بدأ بافاروتي حياته كتينور في إيطاليا عام 1961، ثم بدأ الغناء في دور الأوبرا فيهولندا و فيينا ولندنوأنقرةوبودابستوبرشلونة.وقد اكتسب التينور الشاب حينها الخبرة القيمة بالإضافة إلى التقدير الواضح.وفى</t>
   </si>
   <si>
     <t>"تبدأ الغرفة التجارية الصناعية في محافظة الأحساء تنفيذ برامجها التدريبيةالنسائية اعتباراً من يوم الأحد المقبل وذلك من خلال برنامجين نسائيين بعنوان""فنون التعامل مع الزوج"" وذلك في الفترة من 7 - 8 من شهر ربيع الثاني الحالي،والبرنامج الآخر ""الحب وحده لا يكفي للأبناء"" وذلك في الفترة 9 -10 من شهر ربيعالثاني الحالي، وتقدمهما الدكتورة وداد العيسى من دولة الكويت في مقر الغرفةبمدينة المبرز التابعة للأحساء. وأوضح مدير التدريب والتطوير بالغرفة بدر الحليبي أن المحاضرة ستتناول فيالبرنامج الأول دراسة لأفضل توافق زواجي في العالم، ومظاهر الأسرة السعيدة،ومكونات الزواج السعيد وغير السعيد، وكيف تقيمين علاقاتك الزوجية، والحاجاتالعاطفية المطلوبة في الزواج، وقواعد تحسين العلاقة الزوجية، بالإضافة إلى مهاراتالاتصال بين الزوجين، وفنون التحدث والاستماع، ومهارات حل النزاعات بين الزوجين. كما تتناول عده محاور في البرنامج الآخر ومن أبرزها التواصل الإيجابي معالأبناء، وعناصر الاتصال مع الأبناء، وتصنيف الدراسات لأنماط شخصية الأبناء،وكيفية الحوار مع الأبناء، وكيف نثق في أنفسنا وفي الأبناء، وكيف نربي الثقة عندالأبناء، وكيف تكسب الأم صداقة ابنها، بالإضافة إلى أسباب المشاكل مع الأبناء،ومهارات حل مشكلات الأبناء."</t>
@@ -150,16 +150,46 @@
     <t>"تبدأ الغرفة التجارية الصناعية في محافظة الأحساء تنفيذ برامجها التدريبيةالنسائية اعتباراً من يوم الأحد المقبل وذلك من خلال برنامجين نسائيين بعنوان""فنون التعامل مع الزوج"" وذلك في الفترة من 7 - 8 من شهر ربيع الثاني الحالي،والبرنامج الآخر ""الحب وحده لا يكفي للأبناء"" وذلك في الفترة 9 -10 من شهر ربيعالثاني الحالي، وتقدمهما الدكتورة وداد العيسى من دولة الكويت في مقر الغرفةبمدينة المبرز التابعة للأحساء.</t>
   </si>
   <si>
-    <t>TextRank</t>
-  </si>
-  <si>
-    <t>Recall</t>
-  </si>
-  <si>
-    <t>Precision</t>
-  </si>
-  <si>
-    <t>FScore</t>
+    <t>" _طرح مدير مدرسة حبيب بن زيد الأنصاري الابتدائية برنامجا هو الأول من نوعه علىمستوى منطقة المدينة المنورة التعليمية</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> إن لم يكن الأول من نوعه على مستوىالسعودية على حسب تصريحه</t>
+  </si>
+  <si>
+    <t>" يشكل الإصلاح  في العالم العربي أحد أهم محاور المنتدى الاقتصادي العالمي الذييتخلى عن نخبويته لأول مرة ليرتكز في حوارا ته حوله إلى استطلاعات رأي تخاطب نبضالشارع العربي من محيطه إلى خليجة .. . ماذا يريد وما هي أولوياته؟وبانتظار نتائج استفتاء قناة العربية التى ستناقش في ثلاث جلسات عمل الى جانباستطلاع ينفذه معهد غالوب.. ثمة قناعة بدأت تتبلور بان الاصلاح قد بات مطلباذاتيا ملحا يحظى بإجماع يعزل معه الرافضين . في الأردن ثمة ورشة حوارية دائرة في الجامعات وفي الصحافة ومؤسسات المجتمع المدنيهدفها إشراك المجتمع على اختلاف شرائحه لبناء خزان افكار حول عملية الإصلاحبمفهومه الشامل الذي يحتاج لان يبنى  على أرضية صلبة ومؤسسية بشراكة الجميعبقناعة بان نتاج  كل هذا الجهد انما هي مصلحة للجميع وبان أي تعثر انما هومسؤولية وضرر للجميع .. فالشراكة هي التي ينخرط المجتمع بكل فئاته وأجيالهلبنائها .والمفهوم الشامل للاصلاح هو الذي لا يقيد نفسه بجزئية السياسة على اهميتها  لكنهجسد متكامل يضم التعليم والقضاء والاقتصاد والإعلام ..فعند الحديث عن التعليمينبغي أن نقف لنسأل .. هل تضييق الفجوة بين من هو قادر على توفير بيئة ملائمةيتعلم فيها ابنه وبين من لا يستطيع أمر مرفوض..؟ بعد عامين على إدخال اللغة الانجليزية والكمبيوتر الى المدارس العامة .. بالتأكيدهناك فرق ، والا ما معنى ذلك الشغف الذى بات يبديه التلاميذ للتعليم في المدارسالحكومية .. ."" انظر الى ابنك فانك حتما ستلاحظ الفرق "" لكن ما نزال نحتاج الىالكثير . ان التعليم وحده هو الذي يحدث الفرق عندما تحرز ثقافة المجتمع تطوراملموسا وتترسخ مبادىء تكافؤ الفرص بفضله لقد عزز الملك اتجاهات الاصلاح والتحديث باشراف منه ومتابعة حثيثة عبر برنامجاحالها الى استراتيجية تتصدى لها الحكومات المتعاقبة بمعزل عن التوتر الاقليميفقد  قرر ان لا يتريث كما فعل غيره وان لا ينتظر الى ان يحدث الاستقرار السياسيفي المنطقة  على اهميته للبدء بالاصلاحات و نتائج البداية المبكرة قادمة لا ريب ، فالاصلاحات التي ستاخذ من الان نهجا مؤسسيا ستدفع لان يصبح  الاردن نموذجا يحتذىفي المنطقة».  لقد حدد الملك عددا من القضايا التي لا تحتمل التأجيل ولا تقبل التردد منهاتحرير الاقتصاد وتحديثه ورفع مستوى معيشة الاردنيين وتبني سياسات اقتصادية تؤهلالاردن للاندماج بالاقتصاد العالمي، للاستفادة بأكبر قدر ممكن من الفرص المتاحةعلى اساس ابراز المزايا التنافسية التي يتمتع بها الاردن.ان احداث التنمية عملية لا تقتصر على الحكومة وحدها مع دورها الحيوي والاساسي فيتهيئة المناخ الملائم لاطلاقها والعمل بعزم »لزيادة نسبة النمو الاقتصادي وتوفيرفرص العمل للشباب والحد من مشكلتي الفقر والبطالة، بتطوير البرامج التعليميةوربطها بسوق العمل وبرامج التدريب المهني وتبني استراتيجية طموحة لتنميةالمحافظات بمشاركة فاعلة من المجتمعات المحلية».ان مبادرات كثيرة أطلقها الملك اراد معها ان تشكل نماذج يجب على المؤسساتالحكومية والاهلية ان تقتفي آثارها وهي التي لامست عمق حاجات المجتمع وتطلعاتابنائه الى حياة تقوم على الابداع والمبادرة وحفز الانتاج ان نعطي المواطن سنارةتمكنه من صيد دائم افضل من منحه سمكة لمرة واحدة."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ماذا يريد وما هي اولوياته؟وبانتظار نتائج استفتاء قناة العربية التى ستناقش في ثلاث جلسات عمل الى جانباستطلاع ينفذه معهد غالوب. فعند الحديث عن التعليمينبغي ان نقف لنسال .  هل تضييق الفجوة بين من هو قادر على توفير بيئة ملائمةيتعلم فيها ابنه وبين من لا يستطيع امر مرفوض. </t>
+  </si>
+  <si>
+    <t>ان التعليم وحده هو الذي يحدث الفرق عندما تحرز ثقافة المجتمع تطوراملموسا وتترسخ مبادىء تكافؤ الفرص بفضله لقد عزز الملك اتجاهات الاصلاح والتحديث باشراف منه ومتابعة حثيثة عبر برنامجاحالها الى استراتيجية تتصدى لها الحكومات المتعاقبة بمعزل عن التوتر الاقليميفقد  قرر ان لا يتريث كما فعل غيره وان لا ينتظر الى ان يحدث الاستقرار السياسيفي المنطقة  على اهميته للبدء بالاصلاحات و نتائج البداية المبكرة قادمة لا ريب ، فالاصلاحات التي ستاخذ من الان نهجا مؤسسيا ستدفع لان يصبح  الاردن نموذجا يحتذىفي المنطقة».لقد حدد الملك عددا من القضايا التي لا تحتمل التأجيل ولا تقبل التردد منهاتحرير الاقتصاد وتحديثه ورفع مستوى معيشة الاردنيين وتبني سياسات اقتصادية تؤهلالاردن للاندماج بالاقتصاد العالمي، للاستفادة بأكبر قدر ممكن من الفرص المتاحةعلى اساس ابراز المزايا التنافسية التي يتمتع بها الاردن.انمبادرات كثيرة أطلقها الملك اراد معها ان تشكل نماذج يجب على المؤسساتالحكومية والاهلية ان تقتفي آثارها وهي التي لامست عمق حاجات المجتمع وتطلعاتابنائه الى حياة تقوم على الابداع والمبادرة وحفز الانتاج ان نعطي المواطن سنارةتمكنه من صيد دائم افضل من منحه سمكة لمرة واحدة."</t>
+  </si>
+  <si>
+    <t>"تعرف الرياضيات بأنها دراسة القياس و الحساب ؛ هذا بالإضافة إلى المفاهيم الحديثة نسبيا و منها البنية ، الفضاء أو الفراغ ، و التغير و الابعاد. و بشكل عام قد يعرفها البعض على أنها دراسة البنى المجردة باستخدام المنطق و البراهين الرياضية و التدوين الرياضي. و بشكل أكثر عمومية، قد تعرف الرياضيات أيضا على انها دراسة الأعداد و أنماطها.و لقد نشأت الرياضيات بقيام الإنسان بقياس ما يشاهده من ظواهر الطبيعة بناء على فطرة و خاصية في الإنسان ألا و هى اهتمامه بقياس كل ما حوله إلى جانب إحتياجاته العملية فهكذا كان هناك ضرورة لقياس قسمة المقوتة (الطعام) بين أفراد العائلة و قياس الوقت و الفصول و المحاصيل الزراعية تقسيم الأراضى و غنائم الحملات الحربية و المحاسبة للتمكن من الإتجار إلى جانب علم الملاحة بالنجوم في السفر و الترحال للتجارة و الإستكشاف و القياسات اللازمة لتشييد الأبنية و المدن.و هكذا فإن البنى الرياضية التي يدرسها الرياضيون غالبا ما يعود اصلها إلى العلوم الطبيعية، و خاصة علم الطبيعة، ولكن الرياضيين يقومون بتعريف و دراسة بنى اخرى لاغراض رياضية بحتة، لان هذه البنى قد توفر تعميما لحقول اخرى من الرياضيات مثلا، او ان تكون عاملا مساعدا في حسابات معينة، و اخيرا فان الرياضيين قد يدرسون حقولا معينة من الرياضيات لتحمسهم لها، معتبرين ان الرياضيات هي فن و ليس علما تطبيقيا. كان الكتبة البابليون منذ أكثر من 3000 عام يمارسون كتابة الأعداد وحساب الفوائد ولاسيما في الأعمال التجارية ببابل. وكانت الأعداد والعمليات الحسابية تدون فوق ألواح الصلصال بقلم من البوص المدبب. ثم توضع في الفرن لتجف. وكانوا يعرفون الجمع والضرب والطرح والقسمة. ولم يكونوا يستخدمون فيها النظام العشري المتبع حاليا مما زادها صعوبة حيث كانوا يتبعون النظام الستيني الذي يتكون من 60 رمزا للدلالة علي الأعداد من 1-60. وطور قدماء المصريين هذا النظام في مسح الأراضي بعد كل فيضان لتقدير الضرائب. كما كانوا يتبعون النظام العشري وهو العد بالآحاد والعشرات والمئات. لكنهم لم يعرفوا الصفر. لهذا كانوا يكتبون 600بوضع 6رموز يعبر كل رمز على 100."</t>
+  </si>
+  <si>
+    <t>"تعرف الرياضيات بانها دراسة القياس و الحساب ؛ هذا بالاضافة الى المفاهيم الحديثة نسبيا و منها البنية ، الفضاء او الفراغ ، و التغير و الابعاد.  و بشكل عام قد يعرفها البعض على انها دراسة البنى المجردة باستخدام المنطق و البراهين الرياضية و التدوين الرياضي. "</t>
+  </si>
+  <si>
+    <t>"تعرف الرياضيات بأنها دراسة القياس و الحساب ؛ هذا بالإضافة إلى المفاهيم الحديثة نسبيا و منها البنية ، الفضاء أو الفراغ ، و التغير و الابعاد.هكذا فإن البنى الرياضية التي يدرسها الرياضيون غالبا ما يعود اصلها إلى العلوم الطبيعية، و خاصة علم الطبيعة، ولكن الرياضيين يقومون بتعريف و دراسة بنى اخرى لاغراض رياضية بحتة، لان هذه البنى قد توفر تعميما لحقول اخرى من الرياضيات مثلا، او ان تكون عاملا مساعدا في حسابات معينة، و اخيرا فان الرياضيين قد يدرسون حقولا معينة من الرياضيات لتحمسهم لها، معتبرين ان الرياضيات هي فن و ليس علما تطبيقيا.ولم يكونوا يستخدمون فيها النظام العشري المتبع حاليا مما زادها صعوبة حيث كانوا يتبعون النظام الستيني الذي يتكون من 60 رمزا للدلالة علي الأعداد من 1-60.لهذا كانوا يكتبون 600بوضع 6رموز يعبر كل رمز على 100."</t>
+  </si>
+  <si>
+    <t>"الفيزياء لفظ اشتق من اليونانية فيزيكوس اي طبيعي، والكلمة مشتقة من الجذر فيزيس اي طبيعة. الفيزياء هو علم الطبيعة ، فبدءا من الكوارك البالغ الصغر إلى الكون العظيم الممتد ، تحاول الفيزياء صياغة قوانين رياضية تحكم هذا العالم المادي الطبيعي و سبر أغوار تركيب المادة و مكوناتها الأساسية ، و القوى الأساسية التي تتبادلها الجسيمات و الأجسام المادية ، إضافة إلى نتائج هذه القوى. أحيانا في الفيزياء الحديثة تضاف لهذه المجالات دراسة قوانين التناظر و الانحفاظ ، مثل قوانين حفظ الطاقة و الزخم و الشحنة الكهربائية. و لأجل هذا يدرس الفيزيائيون مجالا واسعا من الظواهر الفيزيائية تمتد من المجالات الصغيرة المدى إلى المجالات الواسعة المدى ، و من الجسيمات تحت-ذرية التي تتكون منها جميع المادة الباريونية فيزياء الجسيمات إلى درساة سلوك الأجسام الفيزيائية في العالم الكلاسيكي إلى دراسة حركة النجوم في الفضاء المادي سواء ضمن السرعات العادية أو قريبا من سرعة الضوء و أخيرا دراسة الكون بمجمله.الفيزياء هو علم الطبيعة، تفصيلاً؛ هو فرع من العلوم والذي يهتم باستكشاف وتشخيص القوانين الكونية التي تتحكم في طبيعة المادة و الطاقة والفراغ والزمن. الإستكشافات في الفيزياء لها صدي كبير وتأثير بالغ في العلوم الطبيعية، والفيزياء وصفها العلماء بأنها العلم الأساسي وذلك لأن مجالات العلوم الأخري مثل الكيمياء و علم الأحياء تقوم بتشخيص أنظمة مادية تعتمد خواصها علي قوانين الفيزياء.الفيزياء كعلم تميزت عن الفلسفة الطبيعية مع بداية الثورة العلمية خلال القرنين السادس عشر و السابع عشر، وظلت هكذا حتي أشرق فجر الفيزياء الحديثة مع بداية القرن العشرين. استمر المجال في التوسع بسبب مجموعة متنامية من البحوث التي أدت ألي استكشافات ثورية مثل وضع النموذج المثالي لحركة الجسيمات الرئيسية أي النواة وما حولها من الإليكترونات، وكذلك وضع بحث لتاريخ الكون بالتفصيل، حتي وصلت إلى الطاقة النووية وأشباه الموصلات اللتين أحدثتا ثورة عظيمة في عالم التكنولوجيا.أما الآن في هذه البحوث تجري لإحداث تقدم في مجالات التوصيل الفائق الحوسبة الكمومية وذلك في حالة الدرجات العالية. بناءا علي الملاحظة والتجربة والنظريات العميقة بعيدة المدي فإن الفيزياء قدمت العديد من الإسهامات في مجال العلوم و التكنولوجيا والفلسفة ."</t>
+  </si>
+  <si>
+    <t>"الفيزياء لفظ اشتق من اليونانية فيزيكوس اي طبيعي، والكلمة مشتقة من الجذر فيزيس اي طبيعة.  و لاجل هذا يدرس الفيزيائيون مجالا واسعا من الظواهر الفيزيائية تمتد من المجالات الصغيرة المدى الى المجالات الواسعة المدى ، و من الجسيمات تحت-ذرية التي تتكون منها جميع المادة الباريونية فيزياء الجسيمات الى درساة سلوك الاجسام الفيزيائية في العالم الكلاسيكي . الفيزياء كعلم تميزت عن الفلسفة الطبيعية مع بداية الثورة العلمية خلال القرنين السادس عشر و السابع عشر، وظلت هكذا حتي اشرق فجر الفيزياء الحديثة مع بداية القرن العشرين. "</t>
+  </si>
+  <si>
+    <t>و لأجل هذا يدرس الفيزيائيون مجالا واسعا من الظواهر الفيزيائية تمتد من المجالات الصغيرة المدى إلى المجالات الواسعة المدى ، و من الجسيمات تحت-ذرية التي تتكون منها جميع المادة الباريونية فيزياء الجسيمات إلى درساة سلوك الأجسام الفيزيائية في العالم الكلاسيكي إلى دراسة حركة النجوم في الفضاء المادي سواء ضمن السرعات العادية أو قريبا من سرعة الضوء و أخيرا دراسة الكون بمجمله.الفيزياءكعلم تميزت عن الفلسفة الطبيعية مع بداية الثورة العلمية خلال القرنين السادس عشر و السابع عشر، وظلت هكذا حتي أشرق فجر الفيزياء الحديثة مع بداية القرن العشرين.استمر المجال في التوسع بسبب مجموعة متنامية من البحوث التي أدت ألي استكشافات ثورية مثل وضع النموذج المثالي لحركة الجسيمات الرئيسية أي النواة وما حولها من الإليكترونات، وكذلك وضع بحث لتاريخ الكون بالتفصيل، حتي وصلت إلى الطاقة النووية وأشباه الموصلات اللتين أحدثتا ثورة عظيمة في عالم التكنولوجيا.أما</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"علم الاحياء أو البيولوجيا من اليونانية،  Biosتعني الحياة و Logos تعني المقالة أو الدراسة هو علم دراسة الحياة  و الكائنات الحية من حيث بنيتها، و طبيعتها، و صفاتها، و أنواعها، و القوانين التي تحكم طرق عيشها و تطورها و تفاعلها  مع وسطها الطبيعي.و علم الاحياء واسع جدا و ينقسم لعدة فروع من أهمها علم الكائنات المجهرية و علم الحيوان و علم النبات و كذلك علم  وضائف الاعضاء و الكيمياء الحيوية و علم البيئة. و مع ترقي هذا العلم، منذ القرن التاسع عشر، صار ذات صلات وثيقة  بالعلوم أخرى، النظرية منها و التطبيقية، مثل الطب و الصيدلة و مجالات تقنية أخرى تلبي إحتياجات الإنسان الضرورية  والمستمرة. و هكذا صرنا اليوم لا نتحدث عن علم بل علوم الحياة .يتعامل علم الأحياء مع دراسة كافة أشكال الحياة . حيث يهتم بخصائص المتعضيات الحية و تصنيفها و سلوكها ، كما يدرس  كيفية ظهور هذه الأنواع إلى الوجود و العلاقات المتبادلة بين بعضها البعض و بينها و بين بيئتها . لذلك فإن علم الأحياء  يحتضن داخله العديد من التخصصات و الفروع العلمية المستقلة . لكنها جميعا تجتمع في علاقتها بالكائنات الحية ظاهرة  الحياة على مجال واسع من الأنواع و الحجام تبدا بدراسة الفيروسات و الجراثيم ثم النباتات و الحيوانات ، في حين تختص  فروع اخرى بدراسة العمليات الحيوية ضمن الخلية مثل الكيمياء الحيوية إلى فروع دراسة العلاقات بين الحياء و البيئة في  علم البيئة.على مستوى العضوية ، تأخذ البيولوجيا على عاتقها دراسة ظواهر مثل الولادة ، النمو ، الشيخوخة aging ، الموت   death و تفسخ الكائات الحية ، ناهيك عن التشابهات بين الأجيال offspring و آبائهم وراثة   heredity  كما يدرس أيضا ازهرار النباتات و غيرها من الظواهر حيرت الإنسانية خلال التاريخ .ظواره أخرى مثل إفراز الحليب lactation ، metamorphosis ، وضع البيض ، تشافي  healing ، الانتحاء Tropism . ضمن مجال أوسع من الوقت و المكان ، يدرس علماء الأحياء تهجين  الحيوانات و النباتات ، إضافة للتنوع الهائل في الحياة النباتية و الحيوانية التنوع الحيوي biodiversity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  التغير في العضويات الحية عبر الزمن التطور </t>
+  </si>
+  <si>
+    <t>"علم الاحياء أو البيولوجيا من اليونانية،  Biosتعني الحياة و Logos تعني المقالة أو الدراسة هو علم دراسة الحياة  و الكائنات الحية من حيث بنيتها، و طبيعتها، و صفاتها، و أنواعها، و القوانين التي تحكم طرق عيشها و تطورها و تفاعلها  مع وسطها الطبيعي.وعلم الاحياء واسع جدا و ينقسم لعدة فروع من أهمها علم الكائنات المجهرية و علم الحيوان و علم النبات و كذلك علم  وضائف الاعضاء و الكيمياء الحيوية و علم البيئة.لكنها جميعا تجتمع في علاقتها بالكائنات الحية ظاهرة  الحياة على مجال واسع من الأنواع و الحجام تبدا بدراسة الفيروسات و الجراثيم ثم النباتات و الحيوانات ، في حين تختص  فروع اخرى بدراسة العمليات الحيوية ضمن الخلية مثل الكيمياء الحيوية إلى فروع دراسة العلاقات بين الحياء و البيئة في  علم البيئة.على</t>
   </si>
 </sst>
 </file>
@@ -204,7 +234,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -250,22 +280,22 @@
         <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6000000238418579</v>
+        <v>0.20000000298023224</v>
       </c>
       <c r="E2" t="n">
-        <v>0.27272728085517883</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3750000298023224</v>
+        <v>0.13333334028720856</v>
       </c>
       <c r="G2" t="n">
-        <v>0.25</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.10000000149011612</v>
+        <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1428571492433548</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -424,13 +454,13 @@
         <v>32</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E8" t="n">
-        <v>0.25</v>
+        <v>0.27272728085517883</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3333333432674408</v>
+        <v>0.40000003576278687</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -514,10 +544,10 @@
         <v>1.0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3333333432674408</v>
+        <v>0.25</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5</v>
+        <v>0.4000000059604645</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -555,6 +585,151 @@
         <v>0.0</v>
       </c>
       <c r="I12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.3333333432674408</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.3333333432674408</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.2857142686843872</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I17" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -565,7 +740,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -585,48 +760,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.24772726405750622</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.03571428494019942</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.13715383139523593</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.03181818127632141</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.15971166437322443</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.02951593832536177</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>